<commit_message>
Change in summary statistics
After finding the results I realized the previous summary statistics did not work as the basis for the results. This code creates new tables for mothers and children.
</commit_message>
<xml_diff>
--- a/Outputs/Summary statistics.xlsx
+++ b/Outputs/Summary statistics.xlsx
@@ -10,7 +10,7 @@
   </mc:AlternateContent>
   <xr:revisionPtr revIDLastSave="617" documentId="8_{86E410C8-AB74-4262-A871-DD752183BDC4}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{D7F2AC14-6FD8-4D32-904F-BE2379779910}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{1F6A4B9F-4C35-4DA5-A84E-0F6D7B1E5A7E}"/>
+    <workbookView xWindow="5760" yWindow="3396" windowWidth="17280" windowHeight="8964" xr2:uid="{1F6A4B9F-4C35-4DA5-A84E-0F6D7B1E5A7E}"/>
   </bookViews>
   <sheets>
     <sheet name="Summary" sheetId="7" r:id="rId1"/>
@@ -971,6 +971,51 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="20" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="15" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="3" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="3" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="13" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="3" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="20" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
@@ -983,49 +1028,13 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="20" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="3" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="3" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="3" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="15" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="13" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="16" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -1037,17 +1046,8 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="14" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="2" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="6">
@@ -2589,8 +2589,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E13E6BC4-C2C0-4683-8130-1201DDCDC7E8}">
   <dimension ref="A1:O63"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A36" workbookViewId="0">
-      <selection activeCell="M49" sqref="M49"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A37" workbookViewId="0">
+      <selection activeCell="A40" sqref="A40:G40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2607,13 +2607,13 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:15" ht="18" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="102" t="s">
+      <c r="A1" s="111" t="s">
         <v>6</v>
       </c>
-      <c r="B1" s="102"/>
-      <c r="C1" s="102"/>
-      <c r="D1" s="102"/>
-      <c r="E1" s="102"/>
+      <c r="B1" s="111"/>
+      <c r="C1" s="111"/>
+      <c r="D1" s="111"/>
+      <c r="E1" s="111"/>
     </row>
     <row r="2" spans="1:15" ht="17.399999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A2" s="76" t="s">
@@ -2631,7 +2631,7 @@
       <c r="E2" s="78"/>
     </row>
     <row r="3" spans="1:15" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A3" s="108" t="s">
+      <c r="A3" s="109" t="s">
         <v>30</v>
       </c>
       <c r="B3" s="82">
@@ -2649,7 +2649,7 @@
       <c r="E3" s="78"/>
     </row>
     <row r="4" spans="1:15" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A4" s="109"/>
+      <c r="A4" s="112"/>
       <c r="B4" s="83" t="str">
         <f>"("&amp;ROUND('[1]2002_house'!$E$5,0)&amp;")"</f>
         <v>(53824)</v>
@@ -2665,7 +2665,7 @@
       <c r="E4" s="78"/>
     </row>
     <row r="5" spans="1:15" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A5" s="109" t="s">
+      <c r="A5" s="112" t="s">
         <v>29</v>
       </c>
       <c r="B5" s="82">
@@ -2689,7 +2689,7 @@
       <c r="N5"/>
     </row>
     <row r="6" spans="1:15" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A6" s="109"/>
+      <c r="A6" s="112"/>
       <c r="B6" s="82" t="str">
         <f>"("&amp;ROUND('[1]2002_house'!$E$10,0)&amp;")"</f>
         <v>(16808)</v>
@@ -2711,7 +2711,7 @@
       <c r="N6"/>
     </row>
     <row r="7" spans="1:15" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A7" s="109" t="s">
+      <c r="A7" s="112" t="s">
         <v>2</v>
       </c>
       <c r="B7" s="84">
@@ -2729,7 +2729,7 @@
       <c r="E7" s="78"/>
     </row>
     <row r="8" spans="1:15" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A8" s="109"/>
+      <c r="A8" s="112"/>
       <c r="B8" s="84" t="str">
         <f>"("&amp;ROUND('[1]2002_house'!$E$8,2)&amp;")"</f>
         <v>(2.04)</v>
@@ -2745,7 +2745,7 @@
       <c r="E8" s="78"/>
     </row>
     <row r="9" spans="1:15" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A9" s="109" t="s">
+      <c r="A9" s="112" t="s">
         <v>24</v>
       </c>
       <c r="B9" s="84">
@@ -2763,7 +2763,7 @@
       <c r="E9" s="78"/>
     </row>
     <row r="10" spans="1:15" ht="17.399999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="A10" s="109"/>
+      <c r="A10" s="112"/>
       <c r="B10" s="84" t="str">
         <f>"("&amp;ROUND('[1]2002_house'!$E$7,2)&amp;")"</f>
         <v>(1.6)</v>
@@ -2797,12 +2797,12 @@
       <c r="E11" s="73"/>
     </row>
     <row r="12" spans="1:15" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="110" t="s">
+      <c r="A12" s="108" t="s">
         <v>35</v>
       </c>
-      <c r="B12" s="110"/>
-      <c r="C12" s="110"/>
-      <c r="D12" s="110"/>
+      <c r="B12" s="108"/>
+      <c r="C12" s="108"/>
+      <c r="D12" s="108"/>
       <c r="E12" s="86"/>
       <c r="F12" s="86"/>
       <c r="G12" s="86"/>
@@ -2829,56 +2829,56 @@
       <c r="M13" s="86"/>
     </row>
     <row r="14" spans="1:15" ht="16.8" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A14" s="107" t="s">
+      <c r="A14" s="100" t="s">
         <v>3</v>
       </c>
-      <c r="B14" s="107"/>
-      <c r="C14" s="107"/>
-      <c r="D14" s="107"/>
-      <c r="E14" s="107"/>
-      <c r="F14" s="107"/>
-      <c r="G14" s="107"/>
-      <c r="I14" s="107" t="s">
+      <c r="B14" s="100"/>
+      <c r="C14" s="100"/>
+      <c r="D14" s="100"/>
+      <c r="E14" s="100"/>
+      <c r="F14" s="100"/>
+      <c r="G14" s="100"/>
+      <c r="I14" s="100" t="s">
         <v>19</v>
       </c>
-      <c r="J14" s="107"/>
-      <c r="K14" s="107"/>
-      <c r="L14" s="107"/>
-      <c r="M14" s="107"/>
-      <c r="N14" s="107"/>
-      <c r="O14" s="107"/>
+      <c r="J14" s="100"/>
+      <c r="K14" s="100"/>
+      <c r="L14" s="100"/>
+      <c r="M14" s="100"/>
+      <c r="N14" s="100"/>
+      <c r="O14" s="100"/>
     </row>
     <row r="15" spans="1:15" ht="16.8" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A15" s="6" t="s">
         <v>0</v>
       </c>
-      <c r="B15" s="105">
+      <c r="B15" s="101">
         <v>2002</v>
       </c>
-      <c r="C15" s="106"/>
-      <c r="D15" s="105" t="s">
+      <c r="C15" s="102"/>
+      <c r="D15" s="101" t="s">
         <v>28</v>
       </c>
-      <c r="E15" s="106"/>
-      <c r="F15" s="107" t="s">
+      <c r="E15" s="102"/>
+      <c r="F15" s="100" t="s">
         <v>27</v>
       </c>
-      <c r="G15" s="107"/>
+      <c r="G15" s="100"/>
       <c r="I15" s="6" t="s">
         <v>0</v>
       </c>
-      <c r="J15" s="105">
+      <c r="J15" s="101">
         <v>2002</v>
       </c>
-      <c r="K15" s="106"/>
-      <c r="L15" s="105" t="s">
+      <c r="K15" s="102"/>
+      <c r="L15" s="101" t="s">
         <v>28</v>
       </c>
-      <c r="M15" s="106"/>
-      <c r="N15" s="107" t="s">
+      <c r="M15" s="102"/>
+      <c r="N15" s="100" t="s">
         <v>27</v>
       </c>
-      <c r="O15" s="107"/>
+      <c r="O15" s="100"/>
     </row>
     <row r="16" spans="1:15" ht="25.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A16" s="12"/>
@@ -3928,56 +3928,56 @@
       <c r="M39" s="104"/>
     </row>
     <row r="40" spans="1:15" ht="48.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A40" s="111" t="s">
+      <c r="A40" s="98" t="s">
         <v>16</v>
       </c>
-      <c r="B40" s="111"/>
-      <c r="C40" s="111"/>
-      <c r="D40" s="111"/>
-      <c r="E40" s="111"/>
-      <c r="F40" s="111"/>
-      <c r="G40" s="111"/>
-      <c r="I40" s="111" t="s">
+      <c r="B40" s="98"/>
+      <c r="C40" s="98"/>
+      <c r="D40" s="98"/>
+      <c r="E40" s="98"/>
+      <c r="F40" s="98"/>
+      <c r="G40" s="98"/>
+      <c r="I40" s="98" t="s">
         <v>16</v>
       </c>
-      <c r="J40" s="111"/>
-      <c r="K40" s="111"/>
-      <c r="L40" s="111"/>
-      <c r="M40" s="111"/>
-      <c r="N40" s="111"/>
-      <c r="O40" s="111"/>
+      <c r="J40" s="98"/>
+      <c r="K40" s="98"/>
+      <c r="L40" s="98"/>
+      <c r="M40" s="98"/>
+      <c r="N40" s="98"/>
+      <c r="O40" s="98"/>
     </row>
     <row r="41" spans="1:15" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="42" spans="1:15" ht="18" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A42" s="113" t="s">
+      <c r="A42" s="105" t="s">
         <v>9</v>
       </c>
-      <c r="B42" s="113"/>
-      <c r="C42" s="113"/>
-      <c r="D42" s="113"/>
-      <c r="E42" s="113"/>
-      <c r="F42" s="113"/>
-      <c r="G42" s="113"/>
+      <c r="B42" s="105"/>
+      <c r="C42" s="105"/>
+      <c r="D42" s="105"/>
+      <c r="E42" s="105"/>
+      <c r="F42" s="105"/>
+      <c r="G42" s="105"/>
     </row>
     <row r="43" spans="1:15" ht="18" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A43" s="108" t="s">
+      <c r="A43" s="109" t="s">
         <v>0</v>
       </c>
-      <c r="B43" s="114">
+      <c r="B43" s="106">
         <v>2002</v>
       </c>
-      <c r="C43" s="114"/>
-      <c r="D43" s="114" t="s">
+      <c r="C43" s="106"/>
+      <c r="D43" s="106" t="s">
         <v>28</v>
       </c>
-      <c r="E43" s="114"/>
-      <c r="F43" s="113" t="s">
+      <c r="E43" s="106"/>
+      <c r="F43" s="105" t="s">
         <v>27</v>
       </c>
-      <c r="G43" s="113"/>
+      <c r="G43" s="105"/>
     </row>
     <row r="44" spans="1:15" ht="16.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A44" s="116"/>
+      <c r="A44" s="110"/>
       <c r="B44" s="89" t="s">
         <v>12</v>
       </c>
@@ -3998,7 +3998,7 @@
       </c>
     </row>
     <row r="45" spans="1:15" ht="16.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A45" s="100" t="s">
+      <c r="A45" s="115" t="s">
         <v>31</v>
       </c>
       <c r="B45" s="92">
@@ -4027,7 +4027,7 @@
       </c>
     </row>
     <row r="46" spans="1:15" ht="16.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A46" s="98"/>
+      <c r="A46" s="113"/>
       <c r="B46" s="96" t="str">
         <f>"("&amp;ROUND('[1]2002_child'!$E$10,2)&amp;")"</f>
         <v>(0.5)</v>
@@ -4045,7 +4045,7 @@
       <c r="G46" s="95"/>
     </row>
     <row r="47" spans="1:15" ht="16.2" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A47" s="98" t="s">
+      <c r="A47" s="113" t="s">
         <v>4</v>
       </c>
       <c r="B47" s="61">
@@ -4074,7 +4074,7 @@
       </c>
     </row>
     <row r="48" spans="1:15" ht="16.2" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A48" s="98"/>
+      <c r="A48" s="113"/>
       <c r="B48" s="44" t="str">
         <f>"("&amp;ROUND('[1]2002_child'!$E$11,2)&amp;")"</f>
         <v>(3.96)</v>
@@ -4092,7 +4092,7 @@
       <c r="G48" s="43"/>
     </row>
     <row r="49" spans="1:14" ht="16.2" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A49" s="98" t="s">
+      <c r="A49" s="113" t="s">
         <v>7</v>
       </c>
       <c r="B49" s="47">
@@ -4121,7 +4121,7 @@
       </c>
     </row>
     <row r="50" spans="1:14" ht="16.2" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A50" s="98"/>
+      <c r="A50" s="113"/>
       <c r="B50" s="53" t="str">
         <f>"("&amp;ROUND('[1]2002_child'!$E$17,2)&amp;")"</f>
         <v>(0.14)</v>
@@ -4139,7 +4139,7 @@
       <c r="G50" s="57"/>
     </row>
     <row r="51" spans="1:14" ht="16.2" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A51" s="98" t="s">
+      <c r="A51" s="113" t="s">
         <v>10</v>
       </c>
       <c r="B51" s="47">
@@ -4168,7 +4168,7 @@
       </c>
     </row>
     <row r="52" spans="1:14" ht="16.2" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A52" s="98"/>
+      <c r="A52" s="113"/>
       <c r="B52" s="44" t="str">
         <f>"("&amp;ROUND('[1]2002_child'!$E$16,2)&amp;")"</f>
         <v>(0.26)</v>
@@ -4186,7 +4186,7 @@
       <c r="G52" s="43"/>
     </row>
     <row r="53" spans="1:14" ht="16.2" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A53" s="101" t="s">
+      <c r="A53" s="116" t="s">
         <v>8</v>
       </c>
       <c r="B53" s="58">
@@ -4215,7 +4215,7 @@
       </c>
     </row>
     <row r="54" spans="1:14" ht="16.2" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A54" s="101"/>
+      <c r="A54" s="116"/>
       <c r="B54" s="44" t="str">
         <f>"("&amp;ROUND('[1]2002_child'!$E$18,2)&amp;")"</f>
         <v>(2.26)</v>
@@ -4233,7 +4233,7 @@
       <c r="G54" s="43"/>
     </row>
     <row r="55" spans="1:14" ht="16.2" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A55" s="98" t="s">
+      <c r="A55" s="113" t="s">
         <v>40</v>
       </c>
       <c r="B55" s="62">
@@ -4262,7 +4262,7 @@
       </c>
     </row>
     <row r="56" spans="1:14" ht="16.2" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A56" s="98"/>
+      <c r="A56" s="113"/>
       <c r="B56" s="62" t="str">
         <f>"("&amp;ROUND('[1]2002_child'!$E$22,2)&amp;")"</f>
         <v>(0.21)</v>
@@ -4280,7 +4280,7 @@
       <c r="G56" s="43"/>
     </row>
     <row r="57" spans="1:14" ht="16.2" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A57" s="98" t="s">
+      <c r="A57" s="113" t="s">
         <v>11</v>
       </c>
       <c r="B57" s="53">
@@ -4309,7 +4309,7 @@
       </c>
     </row>
     <row r="58" spans="1:14" ht="16.2" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A58" s="98"/>
+      <c r="A58" s="113"/>
       <c r="B58" s="44" t="str">
         <f>"("&amp;ROUND('[1]2002_child'!$E$19,2)&amp;")"</f>
         <v>(25.73)</v>
@@ -4327,7 +4327,7 @@
       <c r="G58" s="43"/>
     </row>
     <row r="59" spans="1:14" ht="16.2" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A59" s="98" t="s">
+      <c r="A59" s="113" t="s">
         <v>17</v>
       </c>
       <c r="B59" s="53">
@@ -4356,7 +4356,7 @@
       </c>
     </row>
     <row r="60" spans="1:14" ht="16.2" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="A60" s="99"/>
+      <c r="A60" s="114"/>
       <c r="B60" s="68" t="str">
         <f>"("&amp;ROUND('[1]2002_child'!$E$20,2)&amp;")"</f>
         <v>(15.31)</v>
@@ -4374,15 +4374,15 @@
       <c r="G60" s="67"/>
     </row>
     <row r="61" spans="1:14" customFormat="1" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A61" s="110" t="s">
+      <c r="A61" s="108" t="s">
         <v>35</v>
       </c>
-      <c r="B61" s="110"/>
-      <c r="C61" s="110"/>
-      <c r="D61" s="110"/>
-      <c r="E61" s="110"/>
-      <c r="F61" s="110"/>
-      <c r="G61" s="110"/>
+      <c r="B61" s="108"/>
+      <c r="C61" s="108"/>
+      <c r="D61" s="108"/>
+      <c r="E61" s="108"/>
+      <c r="F61" s="108"/>
+      <c r="G61" s="108"/>
       <c r="H61" s="86"/>
       <c r="I61" s="86"/>
       <c r="J61" s="86"/>
@@ -4392,29 +4392,47 @@
       <c r="N61" s="86"/>
     </row>
     <row r="62" spans="1:14" ht="17.399999999999999" x14ac:dyDescent="0.45">
-      <c r="A62" s="115" t="s">
+      <c r="A62" s="107" t="s">
         <v>38</v>
       </c>
-      <c r="B62" s="115"/>
-      <c r="C62" s="115"/>
-      <c r="D62" s="115"/>
-      <c r="E62" s="115"/>
+      <c r="B62" s="107"/>
+      <c r="C62" s="107"/>
+      <c r="D62" s="107"/>
+      <c r="E62" s="107"/>
       <c r="F62" s="78"/>
       <c r="G62" s="78"/>
     </row>
     <row r="63" spans="1:14" ht="45.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A63" s="112" t="s">
+      <c r="A63" s="99" t="s">
         <v>39</v>
       </c>
-      <c r="B63" s="112"/>
-      <c r="C63" s="112"/>
-      <c r="D63" s="112"/>
-      <c r="E63" s="112"/>
-      <c r="F63" s="112"/>
-      <c r="G63" s="112"/>
+      <c r="B63" s="99"/>
+      <c r="C63" s="99"/>
+      <c r="D63" s="99"/>
+      <c r="E63" s="99"/>
+      <c r="F63" s="99"/>
+      <c r="G63" s="99"/>
     </row>
   </sheetData>
   <mergeCells count="34">
+    <mergeCell ref="A59:A60"/>
+    <mergeCell ref="A55:A56"/>
+    <mergeCell ref="A49:A50"/>
+    <mergeCell ref="A45:A46"/>
+    <mergeCell ref="A47:A48"/>
+    <mergeCell ref="A51:A52"/>
+    <mergeCell ref="A53:A54"/>
+    <mergeCell ref="A1:E1"/>
+    <mergeCell ref="A39:E39"/>
+    <mergeCell ref="B15:C15"/>
+    <mergeCell ref="F15:G15"/>
+    <mergeCell ref="D15:E15"/>
+    <mergeCell ref="A14:G14"/>
+    <mergeCell ref="A3:A4"/>
+    <mergeCell ref="A5:A6"/>
+    <mergeCell ref="A7:A8"/>
+    <mergeCell ref="A9:A10"/>
+    <mergeCell ref="A12:D12"/>
     <mergeCell ref="A40:G40"/>
     <mergeCell ref="A63:G63"/>
     <mergeCell ref="I14:O14"/>
@@ -4430,25 +4448,7 @@
     <mergeCell ref="A62:E62"/>
     <mergeCell ref="A61:G61"/>
     <mergeCell ref="A43:A44"/>
-    <mergeCell ref="A1:E1"/>
-    <mergeCell ref="A39:E39"/>
-    <mergeCell ref="B15:C15"/>
-    <mergeCell ref="F15:G15"/>
-    <mergeCell ref="D15:E15"/>
-    <mergeCell ref="A14:G14"/>
-    <mergeCell ref="A3:A4"/>
-    <mergeCell ref="A5:A6"/>
-    <mergeCell ref="A7:A8"/>
-    <mergeCell ref="A9:A10"/>
-    <mergeCell ref="A12:D12"/>
     <mergeCell ref="A57:A58"/>
-    <mergeCell ref="A59:A60"/>
-    <mergeCell ref="A55:A56"/>
-    <mergeCell ref="A49:A50"/>
-    <mergeCell ref="A45:A46"/>
-    <mergeCell ref="A47:A48"/>
-    <mergeCell ref="A51:A52"/>
-    <mergeCell ref="A53:A54"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -4470,74 +4470,74 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:14" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="B1" s="113" t="s">
+      <c r="B1" s="105" t="s">
         <v>33</v>
       </c>
-      <c r="C1" s="113"/>
-      <c r="D1" s="113"/>
-      <c r="E1" s="113"/>
-      <c r="F1" s="113"/>
-      <c r="G1" s="113"/>
-      <c r="H1" s="113"/>
-      <c r="I1" s="113"/>
-      <c r="J1" s="113"/>
-      <c r="K1" s="113"/>
-      <c r="L1" s="113"/>
+      <c r="C1" s="105"/>
+      <c r="D1" s="105"/>
+      <c r="E1" s="105"/>
+      <c r="F1" s="105"/>
+      <c r="G1" s="105"/>
+      <c r="H1" s="105"/>
+      <c r="I1" s="105"/>
+      <c r="J1" s="105"/>
+      <c r="K1" s="105"/>
+      <c r="L1" s="105"/>
       <c r="M1" s="35"/>
       <c r="N1" s="35"/>
     </row>
     <row r="2" spans="2:14" ht="18" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B2" s="117" t="s">
+      <c r="B2" s="120" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="114">
+      <c r="C2" s="106">
         <v>2002</v>
       </c>
-      <c r="D2" s="114"/>
-      <c r="E2" s="114"/>
-      <c r="F2" s="114"/>
-      <c r="G2" s="114" t="s">
+      <c r="D2" s="106"/>
+      <c r="E2" s="106"/>
+      <c r="F2" s="106"/>
+      <c r="G2" s="106" t="s">
         <v>28</v>
       </c>
-      <c r="H2" s="114"/>
-      <c r="I2" s="114"/>
-      <c r="J2" s="114"/>
-      <c r="K2" s="114" t="s">
+      <c r="H2" s="106"/>
+      <c r="I2" s="106"/>
+      <c r="J2" s="106"/>
+      <c r="K2" s="106" t="s">
         <v>27</v>
       </c>
-      <c r="L2" s="114"/>
-      <c r="M2" s="114"/>
-      <c r="N2" s="119"/>
+      <c r="L2" s="106"/>
+      <c r="M2" s="106"/>
+      <c r="N2" s="122"/>
     </row>
     <row r="3" spans="2:14" ht="18" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B3" s="117"/>
-      <c r="C3" s="114" t="s">
+      <c r="B3" s="120"/>
+      <c r="C3" s="106" t="s">
         <v>32</v>
       </c>
-      <c r="D3" s="114"/>
-      <c r="E3" s="114" t="s">
+      <c r="D3" s="106"/>
+      <c r="E3" s="106" t="s">
         <v>1</v>
       </c>
-      <c r="F3" s="114"/>
-      <c r="G3" s="114" t="s">
+      <c r="F3" s="106"/>
+      <c r="G3" s="106" t="s">
         <v>32</v>
       </c>
-      <c r="H3" s="114"/>
-      <c r="I3" s="114" t="s">
+      <c r="H3" s="106"/>
+      <c r="I3" s="106" t="s">
         <v>1</v>
       </c>
-      <c r="J3" s="114"/>
-      <c r="K3" s="114" t="s">
+      <c r="J3" s="106"/>
+      <c r="K3" s="106" t="s">
         <v>32</v>
       </c>
-      <c r="L3" s="114"/>
-      <c r="M3" s="114" t="s">
+      <c r="L3" s="106"/>
+      <c r="M3" s="106" t="s">
         <v>1</v>
       </c>
-      <c r="N3" s="119"/>
+      <c r="N3" s="122"/>
     </row>
     <row r="4" spans="2:14" ht="15.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B4" s="117"/>
+      <c r="B4" s="120"/>
       <c r="C4" s="36" t="s">
         <v>12</v>
       </c>
@@ -4576,7 +4576,7 @@
       </c>
     </row>
     <row r="5" spans="2:14" ht="15.6" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B5" s="109" t="s">
+      <c r="B5" s="112" t="s">
         <v>4</v>
       </c>
       <c r="C5" s="38">
@@ -4629,7 +4629,7 @@
       </c>
     </row>
     <row r="6" spans="2:14" ht="15.6" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B6" s="109"/>
+      <c r="B6" s="112"/>
       <c r="C6" s="44" t="str">
         <f>"("&amp;ROUND('[2]2002_muj'!$E$13,2)&amp;")"</f>
         <v>(14.96)</v>
@@ -4662,7 +4662,7 @@
       <c r="N6" s="43"/>
     </row>
     <row r="7" spans="2:14" ht="15.6" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B7" s="109" t="s">
+      <c r="B7" s="112" t="s">
         <v>22</v>
       </c>
       <c r="C7" s="47">
@@ -4715,7 +4715,7 @@
       </c>
     </row>
     <row r="8" spans="2:14" ht="15.6" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B8" s="109"/>
+      <c r="B8" s="112"/>
       <c r="C8" s="53" t="str">
         <f>"("&amp;ROUND('[2]2002_muj'!$E$19,2)&amp;")"</f>
         <v>(0.46)</v>
@@ -4748,7 +4748,7 @@
       <c r="N8" s="57"/>
     </row>
     <row r="9" spans="2:14" ht="15.6" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B9" s="123" t="s">
+      <c r="B9" s="118" t="s">
         <v>21</v>
       </c>
       <c r="C9" s="47">
@@ -4801,7 +4801,7 @@
       </c>
     </row>
     <row r="10" spans="2:14" ht="15.6" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B10" s="123"/>
+      <c r="B10" s="118"/>
       <c r="C10" s="44" t="str">
         <f>"("&amp;ROUND('[1]2002_muj'!$E$33,2)&amp;")"</f>
         <v>(0.41)</v>
@@ -4834,7 +4834,7 @@
       <c r="N10" s="43"/>
     </row>
     <row r="11" spans="2:14" ht="15.6" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B11" s="109" t="s">
+      <c r="B11" s="112" t="s">
         <v>20</v>
       </c>
       <c r="C11" s="47">
@@ -4887,7 +4887,7 @@
       </c>
     </row>
     <row r="12" spans="2:14" ht="15.6" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B12" s="109"/>
+      <c r="B12" s="112"/>
       <c r="C12" s="44" t="str">
         <f>"("&amp;ROUND('[1]2002_muj'!$E$22,2)&amp;")"</f>
         <v>(0.37)</v>
@@ -4920,7 +4920,7 @@
       <c r="N12" s="43"/>
     </row>
     <row r="13" spans="2:14" ht="15.6" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B13" s="120" t="s">
+      <c r="B13" s="119" t="s">
         <v>26</v>
       </c>
       <c r="C13" s="44">
@@ -4973,7 +4973,7 @@
       </c>
     </row>
     <row r="14" spans="2:14" ht="15.6" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B14" s="120"/>
+      <c r="B14" s="119"/>
       <c r="C14" s="44" t="str">
         <f>+"("&amp;ROUND('[2]2002_muj'!$E$25,0)&amp;")"</f>
         <v>(33408)</v>
@@ -5006,7 +5006,7 @@
       <c r="N14" s="43"/>
     </row>
     <row r="15" spans="2:14" ht="15.6" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B15" s="109" t="s">
+      <c r="B15" s="112" t="s">
         <v>36</v>
       </c>
       <c r="C15" s="58">
@@ -5059,7 +5059,7 @@
       </c>
     </row>
     <row r="16" spans="2:14" ht="15.6" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B16" s="109"/>
+      <c r="B16" s="112"/>
       <c r="C16" s="44" t="str">
         <f>"("&amp;ROUND('[1]2002_muj'!$E$20,2)&amp;")"</f>
         <v>(2.66)</v>
@@ -5092,7 +5092,7 @@
       <c r="N16" s="43"/>
     </row>
     <row r="17" spans="2:14" ht="15.6" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B17" s="109" t="s">
+      <c r="B17" s="112" t="s">
         <v>11</v>
       </c>
       <c r="C17" s="61">
@@ -5145,7 +5145,7 @@
       </c>
     </row>
     <row r="18" spans="2:14" ht="15.6" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B18" s="109"/>
+      <c r="B18" s="112"/>
       <c r="C18" s="44" t="str">
         <f>"("&amp;ROUND('[1]2002_muj'!$E$27,2)&amp;")"</f>
         <v>(7.19)</v>
@@ -5178,7 +5178,7 @@
       <c r="N18" s="43"/>
     </row>
     <row r="19" spans="2:14" ht="15.6" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B19" s="109" t="s">
+      <c r="B19" s="112" t="s">
         <v>17</v>
       </c>
       <c r="C19" s="61">
@@ -5231,7 +5231,7 @@
       </c>
     </row>
     <row r="20" spans="2:14" ht="15.6" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B20" s="109"/>
+      <c r="B20" s="112"/>
       <c r="C20" s="44" t="str">
         <f>"("&amp;ROUND('[1]2002_muj'!$E$28,2)&amp;")"</f>
         <v>(14.1)</v>
@@ -5264,7 +5264,7 @@
       <c r="N20" s="43"/>
     </row>
     <row r="21" spans="2:14" ht="15.6" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B21" s="120" t="s">
+      <c r="B21" s="119" t="s">
         <v>18</v>
       </c>
       <c r="C21" s="62">
@@ -5317,7 +5317,7 @@
       </c>
     </row>
     <row r="22" spans="2:14" ht="15.6" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B22" s="120"/>
+      <c r="B22" s="119"/>
       <c r="C22" s="62" t="str">
         <f>"("&amp;ROUND('[1]2002_muj'!$E$30,2)&amp;")"</f>
         <v>(0.25)</v>
@@ -5350,7 +5350,7 @@
       <c r="N22" s="43"/>
     </row>
     <row r="23" spans="2:14" ht="15.6" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B23" s="120" t="s">
+      <c r="B23" s="119" t="s">
         <v>23</v>
       </c>
       <c r="C23" s="53">
@@ -5403,7 +5403,7 @@
       </c>
     </row>
     <row r="24" spans="2:14" ht="15.6" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B24" s="120"/>
+      <c r="B24" s="119"/>
       <c r="C24" s="44" t="str">
         <f>"("&amp;ROUND('[1]2002_muj'!$E$32,2)&amp;")"</f>
         <v>(2.11)</v>
@@ -5436,7 +5436,7 @@
       <c r="N24" s="43"/>
     </row>
     <row r="25" spans="2:14" ht="15.6" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B25" s="109" t="s">
+      <c r="B25" s="112" t="s">
         <v>25</v>
       </c>
       <c r="C25" s="53">
@@ -5489,7 +5489,7 @@
       </c>
     </row>
     <row r="26" spans="2:14" ht="15.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="B26" s="121"/>
+      <c r="B26" s="123"/>
       <c r="C26" s="68" t="str">
         <f>"("&amp;ROUND('[1]2002_muj'!$E$31,2)&amp;")"</f>
         <v>(2.56)</v>
@@ -5522,32 +5522,32 @@
       <c r="N26" s="72"/>
     </row>
     <row r="27" spans="2:14" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B27" s="110" t="s">
+      <c r="B27" s="108" t="s">
         <v>35</v>
       </c>
-      <c r="C27" s="110"/>
-      <c r="D27" s="110"/>
-      <c r="E27" s="110"/>
-      <c r="F27" s="110"/>
-      <c r="G27" s="110"/>
-      <c r="H27" s="110"/>
-      <c r="I27" s="110"/>
-      <c r="J27" s="110"/>
-      <c r="K27" s="110"/>
-      <c r="L27" s="110"/>
-      <c r="M27" s="110"/>
-      <c r="N27" s="110"/>
+      <c r="C27" s="108"/>
+      <c r="D27" s="108"/>
+      <c r="E27" s="108"/>
+      <c r="F27" s="108"/>
+      <c r="G27" s="108"/>
+      <c r="H27" s="108"/>
+      <c r="I27" s="108"/>
+      <c r="J27" s="108"/>
+      <c r="K27" s="108"/>
+      <c r="L27" s="108"/>
+      <c r="M27" s="108"/>
+      <c r="N27" s="108"/>
     </row>
     <row r="28" spans="2:14" ht="14.4" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="B28" s="122" t="s">
+      <c r="B28" s="117" t="s">
         <v>14</v>
       </c>
-      <c r="C28" s="122"/>
-      <c r="D28" s="122"/>
-      <c r="E28" s="122"/>
-      <c r="F28" s="122"/>
-      <c r="G28" s="122"/>
-      <c r="H28" s="122"/>
+      <c r="C28" s="117"/>
+      <c r="D28" s="117"/>
+      <c r="E28" s="117"/>
+      <c r="F28" s="117"/>
+      <c r="G28" s="117"/>
+      <c r="H28" s="117"/>
       <c r="I28" s="74"/>
       <c r="J28" s="74"/>
       <c r="K28" s="75"/>
@@ -5556,34 +5556,24 @@
       <c r="N28" s="75"/>
     </row>
     <row r="29" spans="2:14" ht="37.200000000000003" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B29" s="118" t="s">
+      <c r="B29" s="121" t="s">
         <v>37</v>
       </c>
-      <c r="C29" s="118"/>
-      <c r="D29" s="118"/>
-      <c r="E29" s="118"/>
-      <c r="F29" s="118"/>
-      <c r="G29" s="118"/>
-      <c r="H29" s="118"/>
-      <c r="I29" s="118"/>
-      <c r="J29" s="118"/>
-      <c r="K29" s="118"/>
-      <c r="L29" s="118"/>
-      <c r="M29" s="118"/>
-      <c r="N29" s="118"/>
+      <c r="C29" s="121"/>
+      <c r="D29" s="121"/>
+      <c r="E29" s="121"/>
+      <c r="F29" s="121"/>
+      <c r="G29" s="121"/>
+      <c r="H29" s="121"/>
+      <c r="I29" s="121"/>
+      <c r="J29" s="121"/>
+      <c r="K29" s="121"/>
+      <c r="L29" s="121"/>
+      <c r="M29" s="121"/>
+      <c r="N29" s="121"/>
     </row>
   </sheetData>
   <mergeCells count="25">
-    <mergeCell ref="B28:H28"/>
-    <mergeCell ref="B9:B10"/>
-    <mergeCell ref="B11:B12"/>
-    <mergeCell ref="B13:B14"/>
-    <mergeCell ref="B5:B6"/>
-    <mergeCell ref="C3:D3"/>
-    <mergeCell ref="E3:F3"/>
-    <mergeCell ref="C2:F2"/>
-    <mergeCell ref="B1:L1"/>
-    <mergeCell ref="B2:B4"/>
     <mergeCell ref="B29:N29"/>
     <mergeCell ref="B27:N27"/>
     <mergeCell ref="G2:J2"/>
@@ -5599,6 +5589,16 @@
     <mergeCell ref="B23:B24"/>
     <mergeCell ref="B25:B26"/>
     <mergeCell ref="B7:B8"/>
+    <mergeCell ref="C3:D3"/>
+    <mergeCell ref="E3:F3"/>
+    <mergeCell ref="C2:F2"/>
+    <mergeCell ref="B1:L1"/>
+    <mergeCell ref="B2:B4"/>
+    <mergeCell ref="B28:H28"/>
+    <mergeCell ref="B9:B10"/>
+    <mergeCell ref="B11:B12"/>
+    <mergeCell ref="B13:B14"/>
+    <mergeCell ref="B5:B6"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>